<commit_message>
Adding search functionality and edit feature
</commit_message>
<xml_diff>
--- a/static/uploads/export_file/export_admin_excel.xlsx
+++ b/static/uploads/export_file/export_admin_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,15 +523,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>static/uploads/profiles/hgadhiya898034354.jpg</t>
+          <t>static/uploads/profiles/hgadhiya89802234.jpg</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8254235942260960</v>
+        <v>1122830980946353</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>hgadhiya898034354</t>
+          <t>hgadhiya89802234</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Gadhiya</t>
+          <t>gadhiya</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -556,12 +556,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>+91 9316727742</t>
+          <t>+1 8927393723</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>+91 9601406607</t>
+          <t>+1 9601406607</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -581,12 +581,12 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>gujarat</t>
+          <t>Noord-Holland</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>Aruba</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -596,97 +596,12 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>01-06-2024 12:09:50</t>
+          <t>01-08-2024 20:28:24</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>01-06-2024 12:09:50</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>static/uploads/profiles/jaypateldevelopment.jpg</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>4287193301647420</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>jaypateldevelopment</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>jay</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>patel</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Jay@#0401</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>+91 9610526172</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>+91 9726163727</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>harshitgadhiya8980@gmail.com</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>ahmedabad</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>ahmedabad</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Curaçao</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Aruba</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>01-06-2024 15:38:20</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>01-06-2024 15:38:20</t>
+          <t>01-08-2024 20:28:24</t>
         </is>
       </c>
     </row>

</xml_diff>